<commit_message>
Add post-processing for realistic price bounds and fluctuations
</commit_message>
<xml_diff>
--- a/ensemble_test_vs_prediction_results.xlsx
+++ b/ensemble_test_vs_prediction_results.xlsx
@@ -478,7 +478,7 @@
         <v>6.593461175553355</v>
       </c>
       <c r="E2" t="n">
-        <v>6.818180392082708</v>
+        <v>6.857917524323606</v>
       </c>
     </row>
     <row r="3">
@@ -495,7 +495,7 @@
         <v>6.439262235272118</v>
       </c>
       <c r="E3" t="n">
-        <v>6.46053401833186</v>
+        <v>6.503119830300792</v>
       </c>
     </row>
     <row r="4">
@@ -512,7 +512,7 @@
         <v>6.097221053941376</v>
       </c>
       <c r="E4" t="n">
-        <v>6.047992307595077</v>
+        <v>6.218080370165573</v>
       </c>
     </row>
     <row r="5">
@@ -529,7 +529,7 @@
         <v>6.137080058761608</v>
       </c>
       <c r="E5" t="n">
-        <v>6.211533002708441</v>
+        <v>6.341921423272087</v>
       </c>
     </row>
     <row r="6">
@@ -546,7 +546,7 @@
         <v>5.940995906376824</v>
       </c>
       <c r="E6" t="n">
-        <v>5.951530324709408</v>
+        <v>5.968444520820012</v>
       </c>
     </row>
     <row r="7">
@@ -563,7 +563,7 @@
         <v>6.147947382190216</v>
       </c>
       <c r="E7" t="n">
-        <v>5.723836695779556</v>
+        <v>5.776644732809495</v>
       </c>
     </row>
     <row r="8">
@@ -580,7 +580,7 @@
         <v>3.857023577751092</v>
       </c>
       <c r="E8" t="n">
-        <v>4.077794244319882</v>
+        <v>4.556109122745393</v>
       </c>
     </row>
     <row r="9">
@@ -597,7 +597,7 @@
         <v>2.729866926971923</v>
       </c>
       <c r="E9" t="n">
-        <v>3.281044575126892</v>
+        <v>3.66639353244369</v>
       </c>
     </row>
     <row r="10">
@@ -614,7 +614,7 @@
         <v>2.596520100897014</v>
       </c>
       <c r="E10" t="n">
-        <v>2.980603295001119</v>
+        <v>3.082808567070776</v>
       </c>
     </row>
     <row r="11">
@@ -631,7 +631,7 @@
         <v>2.627491672828897</v>
       </c>
       <c r="E11" t="n">
-        <v>3.027672747768513</v>
+        <v>3.091707788714488</v>
       </c>
     </row>
     <row r="12">
@@ -648,7 +648,7 @@
         <v>2.681785260362404</v>
       </c>
       <c r="E12" t="n">
-        <v>3.094201641640552</v>
+        <v>3.039115502164408</v>
       </c>
     </row>
     <row r="13">
@@ -665,7 +665,7 @@
         <v>2.794183163152526</v>
       </c>
       <c r="E13" t="n">
-        <v>3.178860618822967</v>
+        <v>3.11801755371366</v>
       </c>
     </row>
     <row r="14">
@@ -682,7 +682,7 @@
         <v>2.858691259160411</v>
       </c>
       <c r="E14" t="n">
-        <v>3.201882861025518</v>
+        <v>3.208169496592049</v>
       </c>
     </row>
     <row r="15">
@@ -699,7 +699,7 @@
         <v>3.000506132174088</v>
       </c>
       <c r="E15" t="n">
-        <v>3.233741029763497</v>
+        <v>3.072004752223021</v>
       </c>
     </row>
     <row r="16">
@@ -716,7 +716,7 @@
         <v>3.375533531938794</v>
       </c>
       <c r="E16" t="n">
-        <v>3.644582485573889</v>
+        <v>3.42123495093697</v>
       </c>
     </row>
     <row r="17">
@@ -733,7 +733,7 @@
         <v>3.149348910229696</v>
       </c>
       <c r="E17" t="n">
-        <v>3.469184485861308</v>
+        <v>3.418196937883507</v>
       </c>
     </row>
     <row r="18">
@@ -750,7 +750,7 @@
         <v>3.031652654773418</v>
       </c>
       <c r="E18" t="n">
-        <v>3.370473844590994</v>
+        <v>3.326729283189561</v>
       </c>
     </row>
     <row r="19">
@@ -767,7 +767,7 @@
         <v>2.855167562355672</v>
       </c>
       <c r="E19" t="n">
-        <v>3.342382160122233</v>
+        <v>3.383011347750638</v>
       </c>
     </row>
     <row r="20">
@@ -784,7 +784,7 @@
         <v>2.923412336153579</v>
       </c>
       <c r="E20" t="n">
-        <v>3.246638900658882</v>
+        <v>3.195954794956731</v>
       </c>
     </row>
     <row r="21">
@@ -801,7 +801,7 @@
         <v>2.298287174202483</v>
       </c>
       <c r="E21" t="n">
-        <v>2.757840524662277</v>
+        <v>2.752190229701109</v>
       </c>
     </row>
     <row r="22">
@@ -818,7 +818,7 @@
         <v>2.401708764092858</v>
       </c>
       <c r="E22" t="n">
-        <v>2.777196130284039</v>
+        <v>2.939456748273071</v>
       </c>
     </row>
     <row r="23">
@@ -835,7 +835,7 @@
         <v>2.550409735274338</v>
       </c>
       <c r="E23" t="n">
-        <v>2.914821833884728</v>
+        <v>2.867299028563491</v>
       </c>
     </row>
     <row r="24">
@@ -852,7 +852,7 @@
         <v>2.827003063488786</v>
       </c>
       <c r="E24" t="n">
-        <v>3.206857354307564</v>
+        <v>3.140089936237962</v>
       </c>
     </row>
     <row r="25">
@@ -869,7 +869,7 @@
         <v>2.977372956949187</v>
       </c>
       <c r="E25" t="n">
-        <v>3.243397033551193</v>
+        <v>3.092905690763107</v>
       </c>
     </row>
     <row r="26">
@@ -886,7 +886,7 @@
         <v>2.556929071227146</v>
       </c>
       <c r="E26" t="n">
-        <v>2.947371462722338</v>
+        <v>2.959371991001731</v>
       </c>
     </row>
     <row r="27">
@@ -903,7 +903,7 @@
         <v>2.813652956912611</v>
       </c>
       <c r="E27" t="n">
-        <v>3.159671884988593</v>
+        <v>3.155688164795017</v>
       </c>
     </row>
     <row r="28">
@@ -920,7 +920,7 @@
         <v>2.773274974816872</v>
       </c>
       <c r="E28" t="n">
-        <v>3.158644595143116</v>
+        <v>3.045540524691801</v>
       </c>
     </row>
     <row r="29">
@@ -937,7 +937,7 @@
         <v>3.050040813517387</v>
       </c>
       <c r="E29" t="n">
-        <v>3.43896179012051</v>
+        <v>3.413056921577232</v>
       </c>
     </row>
     <row r="30">
@@ -954,7 +954,7 @@
         <v>3.446551393056438</v>
       </c>
       <c r="E30" t="n">
-        <v>3.738695179713033</v>
+        <v>3.602665687103285</v>
       </c>
     </row>
     <row r="31">
@@ -971,7 +971,7 @@
         <v>3.928662996247398</v>
       </c>
       <c r="E31" t="n">
-        <v>4.181493868805462</v>
+        <v>4.039625292044262</v>
       </c>
     </row>
     <row r="32">
@@ -988,7 +988,7 @@
         <v>5.075458710015918</v>
       </c>
       <c r="E32" t="n">
-        <v>4.904261919171168</v>
+        <v>4.667291911210431</v>
       </c>
     </row>
     <row r="33">
@@ -1005,7 +1005,7 @@
         <v>5.629956275130179</v>
       </c>
       <c r="E33" t="n">
-        <v>5.513650670600368</v>
+        <v>5.467678370038672</v>
       </c>
     </row>
     <row r="34">
@@ -1022,7 +1022,7 @@
         <v>5.899163573372626</v>
       </c>
       <c r="E34" t="n">
-        <v>5.593627139622104</v>
+        <v>5.515613192695801</v>
       </c>
     </row>
     <row r="35">
@@ -1039,7 +1039,7 @@
         <v>4.020368811374761</v>
       </c>
       <c r="E35" t="n">
-        <v>4.333836196306277</v>
+        <v>4.493179863750797</v>
       </c>
     </row>
     <row r="36">
@@ -1056,7 +1056,7 @@
         <v>4.070512061038412</v>
       </c>
       <c r="E36" t="n">
-        <v>4.314085605104167</v>
+        <v>4.509818410644426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>